<commit_message>
formatTargetText done and cleaned
</commit_message>
<xml_diff>
--- a/10165.xlsx
+++ b/10165.xlsx
@@ -142,6 +142,9 @@
     <t>Mg</t>
   </si>
   <si>
+    <t>^</t>
+  </si>
+  <si>
     <t>Ingrédients médicinaux</t>
   </si>
   <si>
@@ -173,9 +176,6 @@
   </si>
   <si>
     <t>Phosphatidylserine</t>
-  </si>
-  <si>
-    <t>50 mg</t>
   </si>
   <si>
     <t>Phosphatidylsérine</t>
@@ -1996,15 +1996,17 @@
       <c r="D14" t="s" s="46">
         <v>37</v>
       </c>
-      <c r="E14" s="47"/>
+      <c r="E14" t="s" s="46">
+        <v>38</v>
+      </c>
       <c r="F14" t="s" s="43">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G14" t="s" s="44">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H14" t="s" s="46">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I14" s="47"/>
       <c r="J14" s="10"/>
@@ -2012,7 +2014,7 @@
     <row r="15" ht="30" customHeight="1">
       <c r="A15" s="48"/>
       <c r="B15" t="s" s="31">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="49">
         <v>150</v>
@@ -2023,10 +2025,10 @@
       <c r="E15" s="51"/>
       <c r="F15" s="52"/>
       <c r="G15" t="s" s="36">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H15" t="s" s="50">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I15" s="51"/>
       <c r="J15" s="11"/>
@@ -2034,21 +2036,21 @@
     <row r="16" ht="15" customHeight="1">
       <c r="A16" s="48"/>
       <c r="B16" t="s" s="31">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="49">
         <v>50</v>
       </c>
       <c r="D16" t="s" s="50">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E16" s="51"/>
       <c r="F16" s="52"/>
       <c r="G16" t="s" s="53">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H16" t="s" s="50">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I16" s="51"/>
       <c r="J16" s="11"/>
@@ -2056,19 +2058,21 @@
     <row r="17" ht="15" customHeight="1">
       <c r="A17" s="48"/>
       <c r="B17" t="s" s="31">
-        <v>47</v>
-      </c>
-      <c r="C17" t="s" s="50">
         <v>48</v>
       </c>
-      <c r="D17" s="51"/>
+      <c r="C17" s="49">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s" s="50">
+        <v>37</v>
+      </c>
       <c r="E17" s="51"/>
       <c r="F17" s="52"/>
       <c r="G17" t="s" s="53">
         <v>49</v>
       </c>
       <c r="H17" t="s" s="50">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I17" s="51"/>
       <c r="J17" s="11"/>

</xml_diff>